<commit_message>
remove testing xlsx file
</commit_message>
<xml_diff>
--- a/excel-cleaning/inventory.xlsx
+++ b/excel-cleaning/inventory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ducluu/data-pipeline/excel-cleaning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ducluu/data-cleaning-pipeline/excel-cleaning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B183DE3-A095-F14A-BA4F-1FF3BFE8FFB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B47359-6575-7D4C-B600-90F6484D69C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory Page 1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>Part or Item Number</t>
   </si>
@@ -106,13 +106,7 @@
     <t>Some Number</t>
   </si>
   <si>
-    <t>something</t>
-  </si>
-  <si>
     <t>Test_2</t>
-  </si>
-  <si>
-    <t>else</t>
   </si>
   <si>
     <t>tmp</t>
@@ -691,7 +685,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N8" sqref="N8"/>
+      <selection pane="topRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -701,9 +695,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -717,11 +713,11 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>19</v>
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -736,11 +732,11 @@
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>

</xml_diff>